<commit_message>
added 3 new ingredients
</commit_message>
<xml_diff>
--- a/Evaluation.xlsx
+++ b/Evaluation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hm/Documents/opioid_list/opioid_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D86711-111D-1441-8029-A8DC8173FA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD1EA3-97E4-7640-BB17-CB9D0FFEC49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="500" windowWidth="22380" windowHeight="20500" xr2:uid="{0B53AC7D-9A79-FF40-91B4-6DADAAAF0265}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,27 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Positive</t>
   </si>
   <si>
     <t>Negative</t>
-  </si>
-  <si>
-    <t>TP: 2057 (Drugs that match the new list)</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>FN: 0</t>
-  </si>
-  <si>
-    <t>FP: 0</t>
-  </si>
-  <si>
-    <t>TN: 2396</t>
   </si>
 </sst>
 </file>
@@ -407,20 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E09D7BC-72B1-1546-9CDA-2A3777F8E517}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.33203125" customWidth="1"/>
-    <col min="2" max="2" width="65.5" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -428,31 +413,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>2057</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>B2/(B2+C2)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2396</v>
+      </c>
+      <c r="D3">
+        <f>C3/(C3+B3)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>3</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <f>B2/(B2+B3)</f>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>C3/(C2+C3)</f>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>(B2+C3)/(B2+C2+B3+C3)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>